<commit_message>
Week 7 Data Update
</commit_message>
<xml_diff>
--- a/PEAR/kford.xlsx
+++ b/PEAR/kford.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wpars\OneDrive\Documents\Post-School\Family Feud Data\PEAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836AA68C-1F41-4C34-A3B0-40580C194BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C3926B-1916-48E7-9695-A4D2B7A36D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,172 +276,172 @@
     <t>San Diego State</t>
   </si>
   <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>Utah State</t>
+  </si>
+  <si>
+    <t>Wake Forest</t>
+  </si>
+  <si>
+    <t>UConn</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>UCLA</t>
+  </si>
+  <si>
+    <t>Army</t>
+  </si>
+  <si>
+    <t>Oregon State</t>
+  </si>
+  <si>
+    <t>Miami (OH)</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>Western Kentucky</t>
+  </si>
+  <si>
+    <t>Southern Miss</t>
+  </si>
+  <si>
+    <t>San José State</t>
+  </si>
+  <si>
+    <t>Bowling Green</t>
+  </si>
+  <si>
+    <t>Hawai'i</t>
+  </si>
+  <si>
+    <t>Temple</t>
+  </si>
+  <si>
+    <t>South Alabama</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Western Michigan</t>
+  </si>
+  <si>
+    <t>Liberty</t>
+  </si>
+  <si>
+    <t>Air Force</t>
+  </si>
+  <si>
+    <t>Washington State</t>
+  </si>
+  <si>
+    <t>Georgia Southern</t>
+  </si>
+  <si>
+    <t>Jacksonville State</t>
+  </si>
+  <si>
+    <t>Oklahoma State</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Colorado State</t>
+  </si>
+  <si>
+    <t>Northern Illinois</t>
+  </si>
+  <si>
+    <t>App State</t>
+  </si>
+  <si>
+    <t>Coastal Carolina</t>
+  </si>
+  <si>
+    <t>UL Monroe</t>
+  </si>
+  <si>
+    <t>UAB</t>
+  </si>
+  <si>
+    <t>Arkansas State</t>
+  </si>
+  <si>
+    <t>UTEP</t>
+  </si>
+  <si>
+    <t>Florida International</t>
+  </si>
+  <si>
+    <t>Central Michigan</t>
+  </si>
+  <si>
+    <t>Tulsa</t>
+  </si>
+  <si>
+    <t>Missouri State</t>
+  </si>
+  <si>
+    <t>Kennesaw State</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Eastern Michigan</t>
+  </si>
+  <si>
+    <t>Georgia State</t>
+  </si>
+  <si>
+    <t>Sam Houston</t>
+  </si>
+  <si>
+    <t>Ball State</t>
+  </si>
+  <si>
+    <t>New Mexico State</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Middle Tennessee</t>
+  </si>
+  <si>
+    <t>Akron</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Kent State</t>
+  </si>
+  <si>
+    <t>Florida Atlantic</t>
+  </si>
+  <si>
     <t>North Carolina</t>
-  </si>
-  <si>
-    <t>Stanford</t>
-  </si>
-  <si>
-    <t>Utah State</t>
-  </si>
-  <si>
-    <t>Wake Forest</t>
-  </si>
-  <si>
-    <t>UConn</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>UCLA</t>
-  </si>
-  <si>
-    <t>Army</t>
-  </si>
-  <si>
-    <t>Oregon State</t>
-  </si>
-  <si>
-    <t>Miami (OH)</t>
-  </si>
-  <si>
-    <t>Troy</t>
-  </si>
-  <si>
-    <t>Western Kentucky</t>
-  </si>
-  <si>
-    <t>Southern Miss</t>
-  </si>
-  <si>
-    <t>San José State</t>
-  </si>
-  <si>
-    <t>Bowling Green</t>
-  </si>
-  <si>
-    <t>Hawai'i</t>
-  </si>
-  <si>
-    <t>Temple</t>
-  </si>
-  <si>
-    <t>South Alabama</t>
-  </si>
-  <si>
-    <t>Marshall</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t>Buffalo</t>
-  </si>
-  <si>
-    <t>Western Michigan</t>
-  </si>
-  <si>
-    <t>Liberty</t>
-  </si>
-  <si>
-    <t>Air Force</t>
-  </si>
-  <si>
-    <t>Washington State</t>
-  </si>
-  <si>
-    <t>Georgia Southern</t>
-  </si>
-  <si>
-    <t>Jacksonville State</t>
-  </si>
-  <si>
-    <t>Oklahoma State</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>Colorado State</t>
-  </si>
-  <si>
-    <t>Northern Illinois</t>
-  </si>
-  <si>
-    <t>App State</t>
-  </si>
-  <si>
-    <t>Coastal Carolina</t>
-  </si>
-  <si>
-    <t>UL Monroe</t>
-  </si>
-  <si>
-    <t>UAB</t>
-  </si>
-  <si>
-    <t>Arkansas State</t>
-  </si>
-  <si>
-    <t>UTEP</t>
-  </si>
-  <si>
-    <t>Florida International</t>
-  </si>
-  <si>
-    <t>Central Michigan</t>
-  </si>
-  <si>
-    <t>Tulsa</t>
-  </si>
-  <si>
-    <t>Missouri State</t>
-  </si>
-  <si>
-    <t>Kennesaw State</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>Eastern Michigan</t>
-  </si>
-  <si>
-    <t>Georgia State</t>
-  </si>
-  <si>
-    <t>Sam Houston</t>
-  </si>
-  <si>
-    <t>Ball State</t>
-  </si>
-  <si>
-    <t>New Mexico State</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>Middle Tennessee</t>
-  </si>
-  <si>
-    <t>Akron</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Kent State</t>
-  </si>
-  <si>
-    <t>Florida Atlantic</t>
   </si>
 </sst>
 </file>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,7 +783,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>26.4</v>
+        <v>27.3</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -794,7 +794,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>24.3</v>
+        <v>24.9</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -805,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>24.2</v>
+        <v>24.6</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -816,7 +816,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>23.2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -827,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>22.2</v>
+        <v>22.7</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -835,10 +835,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>20.6</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -846,10 +846,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>20.7</v>
+        <v>20.5</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -857,10 +857,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>20.399999999999999</v>
+        <v>20.2</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -868,10 +868,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>19.7</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -882,7 +882,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>19.2</v>
+        <v>19.7</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>18.899999999999999</v>
+        <v>18.2</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -901,10 +901,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>18.2</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -912,10 +912,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>18.2</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>17.2</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -934,10 +934,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>17.2</v>
+        <v>17.3</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B17">
-        <v>17.100000000000001</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -959,7 +959,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>16.5</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -970,7 +970,7 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>15.3</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -978,10 +978,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>14.9</v>
+        <v>15.3</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>14.7</v>
+        <v>14.9</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B22">
-        <v>14.6</v>
+        <v>14.1</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1011,10 +1011,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>14.3</v>
+        <v>13.9</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B24">
-        <v>13.7</v>
+        <v>13.9</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>13.6</v>
+        <v>13.4</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1044,10 +1044,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>13.3</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1055,10 +1055,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>11.6</v>
+        <v>11.5</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1069,7 +1069,7 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>11.3</v>
+        <v>11.4</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B29">
         <v>11.3</v>
@@ -1088,10 +1088,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B30">
-        <v>10.9</v>
+        <v>11.1</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>10.7</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
-        <v>10.6</v>
+        <v>10.5</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1124,7 +1124,7 @@
         <v>34</v>
       </c>
       <c r="B33">
-        <v>10.6</v>
+        <v>10.3</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>9.9</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B36">
-        <v>8.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1165,10 +1165,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37">
-        <v>8.1999999999999993</v>
+        <v>9.4</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1176,10 +1176,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B38">
-        <v>8.1</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1190,7 +1190,7 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <v>8</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1209,10 +1209,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B41">
-        <v>7.7</v>
+        <v>8</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1220,10 +1220,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B42">
-        <v>7.3</v>
+        <v>7.8</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43">
-        <v>6.9</v>
+        <v>7.6</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1242,10 +1242,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1256,7 +1256,7 @@
         <v>46</v>
       </c>
       <c r="B45">
-        <v>6.1</v>
+        <v>7.6</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1267,7 +1267,7 @@
         <v>47</v>
       </c>
       <c r="B46">
-        <v>5.9</v>
+        <v>6.8</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -1275,10 +1275,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B47">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1286,10 +1286,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B48">
-        <v>5.7</v>
+        <v>6.3</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B49">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -1308,10 +1308,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>5.3</v>
+        <v>5.7</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -1319,10 +1319,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>5.6</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -1330,10 +1330,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B52">
-        <v>4.5999999999999996</v>
+        <v>5.3</v>
       </c>
       <c r="C52">
         <v>51</v>
@@ -1341,10 +1341,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B53">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="C53">
         <v>52</v>
@@ -1352,10 +1352,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="C54">
         <v>53</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B55">
-        <v>4.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C55">
         <v>54</v>
@@ -1374,10 +1374,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B56">
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="C56">
         <v>55</v>
@@ -1385,10 +1385,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B57">
-        <v>4</v>
+        <v>3.7</v>
       </c>
       <c r="C57">
         <v>56</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B58">
-        <v>3.9</v>
+        <v>3.3</v>
       </c>
       <c r="C58">
         <v>57</v>
@@ -1407,10 +1407,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B59">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -1421,7 +1421,7 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="C60">
         <v>59</v>
@@ -1429,10 +1429,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B61">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C62">
         <v>61</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B64">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B65">
         <v>2.5</v>
@@ -1487,7 +1487,7 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>1.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C66">
         <v>65</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B67">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="C67">
         <v>66</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B68">
         <v>0.2</v>
@@ -1517,10 +1517,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B69">
-        <v>0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -1528,10 +1528,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70">
-        <v>-0.3</v>
+        <v>-1</v>
       </c>
       <c r="C70">
         <v>69</v>
@@ -1539,10 +1539,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B71">
-        <v>-0.7</v>
+        <v>-1.3</v>
       </c>
       <c r="C71">
         <v>70</v>
@@ -1550,10 +1550,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B72">
-        <v>-0.7</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="C72">
         <v>71</v>
@@ -1561,10 +1561,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73">
-        <v>-1.1000000000000001</v>
+        <v>-2.4</v>
       </c>
       <c r="C73">
         <v>72</v>
@@ -1572,10 +1572,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B74">
-        <v>-1.5</v>
+        <v>-2.6</v>
       </c>
       <c r="C74">
         <v>73</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B75">
-        <v>-1.7</v>
+        <v>-2.7</v>
       </c>
       <c r="C75">
         <v>74</v>
@@ -1594,10 +1594,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B76">
-        <v>-2.4</v>
+        <v>-2.9</v>
       </c>
       <c r="C76">
         <v>75</v>
@@ -1605,10 +1605,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B77">
-        <v>-2.6</v>
+        <v>-3.1</v>
       </c>
       <c r="C77">
         <v>76</v>
@@ -1616,10 +1616,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B78">
-        <v>-3.1</v>
+        <v>-3.2</v>
       </c>
       <c r="C78">
         <v>77</v>
@@ -1627,10 +1627,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B79">
-        <v>-3.5</v>
+        <v>-3.2</v>
       </c>
       <c r="C79">
         <v>78</v>
@@ -1638,10 +1638,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B80">
-        <v>-4</v>
+        <v>-3.7</v>
       </c>
       <c r="C80">
         <v>79</v>
@@ -1649,10 +1649,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B81">
-        <v>-4.7</v>
+        <v>-3.8</v>
       </c>
       <c r="C81">
         <v>80</v>
@@ -1660,10 +1660,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82">
-        <v>-5.2</v>
+        <v>-3.9</v>
       </c>
       <c r="C82">
         <v>81</v>
@@ -1671,10 +1671,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B83">
-        <v>-5.3</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="C83">
         <v>82</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B84">
-        <v>-5.3</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="C84">
         <v>83</v>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B85">
-        <v>-5.6</v>
+        <v>-4.8</v>
       </c>
       <c r="C85">
         <v>84</v>
@@ -1704,10 +1704,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B86">
-        <v>-5.7</v>
+        <v>-5.3</v>
       </c>
       <c r="C86">
         <v>85</v>
@@ -1715,10 +1715,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B87">
-        <v>-6.1</v>
+        <v>-5.8</v>
       </c>
       <c r="C87">
         <v>86</v>
@@ -1726,10 +1726,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B88">
-        <v>-6.2</v>
+        <v>-5.8</v>
       </c>
       <c r="C88">
         <v>87</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B89">
-        <v>-6.3</v>
+        <v>-6.7</v>
       </c>
       <c r="C89">
         <v>88</v>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="B90">
-        <v>-6.9</v>
+        <v>-6.7</v>
       </c>
       <c r="C90">
         <v>89</v>
@@ -1762,7 +1762,7 @@
         <v>92</v>
       </c>
       <c r="B91">
-        <v>-7.2</v>
+        <v>-7.3</v>
       </c>
       <c r="C91">
         <v>90</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>-7.5</v>
+        <v>-7.7</v>
       </c>
       <c r="C92">
         <v>91</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B93">
         <v>-8</v>
@@ -1792,10 +1792,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B94">
-        <v>-8.3000000000000007</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="C94">
         <v>93</v>
@@ -1803,10 +1803,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B95">
-        <v>-8.5</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="C95">
         <v>94</v>
@@ -1814,10 +1814,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B96">
-        <v>-8.8000000000000007</v>
+        <v>-8.3000000000000007</v>
       </c>
       <c r="C96">
         <v>95</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B97">
-        <v>-8.9</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="C97">
         <v>96</v>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>-9.1</v>
@@ -1847,10 +1847,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B99">
-        <v>-9.4</v>
+        <v>-9.1999999999999993</v>
       </c>
       <c r="C99">
         <v>98</v>
@@ -1858,10 +1858,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B100">
-        <v>-9.6</v>
+        <v>-9.4</v>
       </c>
       <c r="C100">
         <v>99</v>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>-9.6999999999999993</v>
+        <v>-9.6</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>-9.8000000000000007</v>
@@ -1894,7 +1894,7 @@
         <v>104</v>
       </c>
       <c r="B103">
-        <v>-9.8000000000000007</v>
+        <v>-10</v>
       </c>
       <c r="C103">
         <v>102</v>
@@ -1902,10 +1902,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B104">
-        <v>-10</v>
+        <v>-10.6</v>
       </c>
       <c r="C104">
         <v>103</v>
@@ -1913,10 +1913,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B105">
-        <v>-10.3</v>
+        <v>-10.8</v>
       </c>
       <c r="C105">
         <v>104</v>
@@ -1924,10 +1924,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B106">
-        <v>-10.4</v>
+        <v>-10.8</v>
       </c>
       <c r="C106">
         <v>105</v>
@@ -1935,10 +1935,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B107">
-        <v>-10.4</v>
+        <v>-10.8</v>
       </c>
       <c r="C107">
         <v>106</v>
@@ -1946,10 +1946,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B108">
-        <v>-10.6</v>
+        <v>-10.9</v>
       </c>
       <c r="C108">
         <v>107</v>
@@ -1957,10 +1957,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B109">
-        <v>-10.9</v>
+        <v>-11.6</v>
       </c>
       <c r="C109">
         <v>108</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B110">
-        <v>-11.3</v>
+        <v>-11.8</v>
       </c>
       <c r="C110">
         <v>109</v>
@@ -1979,10 +1979,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B111">
-        <v>-11.3</v>
+        <v>-11.9</v>
       </c>
       <c r="C111">
         <v>110</v>
@@ -1990,10 +1990,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B112">
-        <v>-11.5</v>
+        <v>-12.3</v>
       </c>
       <c r="C112">
         <v>111</v>
@@ -2001,10 +2001,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B113">
-        <v>-11.7</v>
+        <v>-13</v>
       </c>
       <c r="C113">
         <v>112</v>
@@ -2012,10 +2012,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B114">
-        <v>-11.8</v>
+        <v>-13</v>
       </c>
       <c r="C114">
         <v>113</v>
@@ -2023,10 +2023,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B115">
-        <v>-12.8</v>
+        <v>-13</v>
       </c>
       <c r="C115">
         <v>114</v>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B116">
-        <v>-13.1</v>
+        <v>-13.4</v>
       </c>
       <c r="C116">
         <v>115</v>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B117">
-        <v>-13.3</v>
+        <v>-13.5</v>
       </c>
       <c r="C117">
         <v>116</v>
@@ -2056,10 +2056,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B118">
-        <v>-14.4</v>
+        <v>-15.2</v>
       </c>
       <c r="C118">
         <v>117</v>
@@ -2067,10 +2067,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B119">
-        <v>-14.4</v>
+        <v>-15.5</v>
       </c>
       <c r="C119">
         <v>118</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B120">
-        <v>-14.6</v>
+        <v>-15.5</v>
       </c>
       <c r="C120">
         <v>119</v>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B121">
-        <v>-14.7</v>
+        <v>-15.6</v>
       </c>
       <c r="C121">
         <v>120</v>
@@ -2100,10 +2100,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B122">
-        <v>-14.9</v>
+        <v>-15.9</v>
       </c>
       <c r="C122">
         <v>121</v>
@@ -2111,10 +2111,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B123">
-        <v>-14.9</v>
+        <v>-16</v>
       </c>
       <c r="C123">
         <v>122</v>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B124">
-        <v>-15.7</v>
+        <v>-16</v>
       </c>
       <c r="C124">
         <v>123</v>
@@ -2136,7 +2136,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>-15.8</v>
+        <v>-16.2</v>
       </c>
       <c r="C125">
         <v>124</v>
@@ -2144,10 +2144,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B126">
-        <v>-16.5</v>
+        <v>-16.8</v>
       </c>
       <c r="C126">
         <v>125</v>
@@ -2155,10 +2155,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B127">
-        <v>-17.399999999999999</v>
+        <v>-17.3</v>
       </c>
       <c r="C127">
         <v>126</v>
@@ -2166,10 +2166,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B128">
-        <v>-18.100000000000001</v>
+        <v>-17.399999999999999</v>
       </c>
       <c r="C128">
         <v>127</v>
@@ -2177,10 +2177,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B129">
-        <v>-18.5</v>
+        <v>-17.7</v>
       </c>
       <c r="C129">
         <v>128</v>
@@ -2188,10 +2188,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B130">
-        <v>-19.3</v>
+        <v>-17.899999999999999</v>
       </c>
       <c r="C130">
         <v>129</v>
@@ -2199,10 +2199,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B131">
-        <v>-20.2</v>
+        <v>-18.600000000000001</v>
       </c>
       <c r="C131">
         <v>130</v>
@@ -2210,7 +2210,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B132">
         <v>-20.5</v>
@@ -2224,7 +2224,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>-20.9</v>
+        <v>-20.8</v>
       </c>
       <c r="C133">
         <v>132</v>
@@ -2232,10 +2232,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B134">
-        <v>-20.9</v>
+        <v>-21</v>
       </c>
       <c r="C134">
         <v>133</v>
@@ -2243,10 +2243,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B135">
-        <v>-21</v>
+        <v>-22.1</v>
       </c>
       <c r="C135">
         <v>134</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136">
-        <v>-25.5</v>
+        <v>-26.2</v>
       </c>
       <c r="C136">
         <v>135</v>
@@ -2265,10 +2265,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B137">
-        <v>-26.4</v>
+        <v>-26.3</v>
       </c>
       <c r="C137">
         <v>136</v>

</xml_diff>

<commit_message>
Week 8 Data Update
</commit_message>
<xml_diff>
--- a/PEAR/kford.xlsx
+++ b/PEAR/kford.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wpars\OneDrive\Documents\Post-School\Family Feud Data\PEAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C3926B-1916-48E7-9695-A4D2B7A36D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCB4AF3-EC23-4EA8-B369-D53D17A077AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -761,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,7 +794,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>27.3</v>
+        <v>28.1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -791,10 +802,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>24.9</v>
+        <v>24.2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -802,10 +813,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>24.6</v>
+        <v>24.1</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -813,10 +824,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>23.2</v>
+        <v>23.7</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -824,10 +835,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>22.7</v>
+        <v>22.5</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -835,10 +846,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>20.6</v>
+        <v>22.1</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -849,7 +860,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>20.5</v>
+        <v>21.4</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -857,10 +868,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>20.2</v>
+        <v>21.1</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -868,10 +879,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>20.100000000000001</v>
+        <v>21.1</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -879,10 +890,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>19.7</v>
+        <v>19.5</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -890,10 +901,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12">
-        <v>18.2</v>
+        <v>18.8</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -901,10 +912,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B13">
-        <v>18.100000000000001</v>
+        <v>18.3</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -915,7 +926,7 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>18.100000000000001</v>
+        <v>17.5</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -923,10 +934,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>17.899999999999999</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -934,10 +945,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>17.3</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -945,10 +956,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>16.600000000000001</v>
+        <v>15.6</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -959,7 +970,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>16.399999999999999</v>
+        <v>15.5</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -967,10 +978,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19">
-        <v>15.3</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -978,10 +989,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>15.3</v>
+        <v>14.9</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -989,10 +1000,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>14.9</v>
+        <v>14.8</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1000,10 +1011,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B22">
-        <v>14.1</v>
+        <v>13.9</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1011,10 +1022,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B23">
-        <v>13.9</v>
+        <v>13.5</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1025,7 +1036,7 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>13.9</v>
+        <v>13.4</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1033,7 +1044,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>13.4</v>
@@ -1044,10 +1055,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1055,10 +1066,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>11.5</v>
+        <v>13.1</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1066,10 +1077,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B28">
-        <v>11.4</v>
+        <v>12.8</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1077,10 +1088,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B29">
-        <v>11.3</v>
+        <v>12.1</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1088,10 +1099,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B30">
-        <v>11.1</v>
+        <v>11.4</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1099,10 +1110,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>10.7</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1110,10 +1121,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B32">
-        <v>10.5</v>
+        <v>10.1</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1121,10 +1132,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>10.3</v>
+        <v>10</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1132,7 +1143,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B34">
         <v>9.9</v>
@@ -1143,10 +1154,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B35">
-        <v>9.8000000000000007</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1154,10 +1165,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B36">
-        <v>9.8000000000000007</v>
+        <v>9.4</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1168,7 +1179,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>9.4</v>
+        <v>9.1</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1176,10 +1187,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B38">
-        <v>9.3000000000000007</v>
+        <v>8.9</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1187,10 +1198,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B39">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1198,10 +1209,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B40">
-        <v>8.3000000000000007</v>
+        <v>8.4</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1209,10 +1220,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1220,10 +1231,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B42">
-        <v>7.8</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1231,10 +1242,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B43">
-        <v>7.6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1242,10 +1253,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B44">
-        <v>7.6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1253,10 +1264,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>7.6</v>
+        <v>7.7</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1264,10 +1275,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B46">
-        <v>6.8</v>
+        <v>7.6</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -1275,10 +1286,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B47">
-        <v>6.8</v>
+        <v>7.6</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1286,10 +1297,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B48">
-        <v>6.3</v>
+        <v>6.6</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -1297,10 +1308,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -1308,10 +1319,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B50">
-        <v>5.7</v>
+        <v>5.3</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -1319,10 +1330,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51">
-        <v>5.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -1330,10 +1341,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B52">
-        <v>5.3</v>
+        <v>4.2</v>
       </c>
       <c r="C52">
         <v>51</v>
@@ -1341,10 +1352,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B53">
-        <v>4.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C53">
         <v>52</v>
@@ -1352,10 +1363,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B54">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="C54">
         <v>53</v>
@@ -1363,10 +1374,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B55">
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="C55">
         <v>54</v>
@@ -1377,7 +1388,7 @@
         <v>63</v>
       </c>
       <c r="B56">
-        <v>4</v>
+        <v>3.7</v>
       </c>
       <c r="C56">
         <v>55</v>
@@ -1388,7 +1399,7 @@
         <v>54</v>
       </c>
       <c r="B57">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="C57">
         <v>56</v>
@@ -1396,10 +1407,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B58">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="C58">
         <v>57</v>
@@ -1407,10 +1418,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B59">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -1421,7 +1432,7 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="C60">
         <v>59</v>
@@ -1429,10 +1440,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -1440,10 +1451,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B62">
-        <v>2.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C62">
         <v>61</v>
@@ -1451,10 +1462,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B63">
-        <v>2.6</v>
+        <v>1.8</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -1462,10 +1473,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B64">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -1473,10 +1484,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B65">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="C65">
         <v>64</v>
@@ -1484,10 +1495,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B66">
-        <v>2.2999999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="C66">
         <v>65</v>
@@ -1495,10 +1506,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B67">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C67">
         <v>66</v>
@@ -1506,10 +1517,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C68">
         <v>67</v>
@@ -1517,10 +1528,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B69">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -1528,10 +1539,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B70">
-        <v>-1</v>
+        <v>-0.7</v>
       </c>
       <c r="C70">
         <v>69</v>
@@ -1539,10 +1550,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B71">
-        <v>-1.3</v>
+        <v>-0.7</v>
       </c>
       <c r="C71">
         <v>70</v>
@@ -1550,10 +1561,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B72">
-        <v>-2.2000000000000002</v>
+        <v>-0.9</v>
       </c>
       <c r="C72">
         <v>71</v>
@@ -1561,10 +1572,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B73">
-        <v>-2.4</v>
+        <v>-1</v>
       </c>
       <c r="C73">
         <v>72</v>
@@ -1572,10 +1583,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B74">
-        <v>-2.6</v>
+        <v>-1</v>
       </c>
       <c r="C74">
         <v>73</v>
@@ -1583,10 +1594,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B75">
-        <v>-2.7</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="C75">
         <v>74</v>
@@ -1597,7 +1608,7 @@
         <v>81</v>
       </c>
       <c r="B76">
-        <v>-2.9</v>
+        <v>-2.7</v>
       </c>
       <c r="C76">
         <v>75</v>
@@ -1605,10 +1616,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B77">
-        <v>-3.1</v>
+        <v>-3</v>
       </c>
       <c r="C77">
         <v>76</v>
@@ -1616,7 +1627,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B78">
         <v>-3.2</v>
@@ -1627,10 +1638,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B79">
-        <v>-3.2</v>
+        <v>-3.7</v>
       </c>
       <c r="C79">
         <v>78</v>
@@ -1638,10 +1649,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B80">
-        <v>-3.7</v>
+        <v>-3.9</v>
       </c>
       <c r="C80">
         <v>79</v>
@@ -1649,10 +1660,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B81">
-        <v>-3.8</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="C81">
         <v>80</v>
@@ -1660,10 +1671,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B82">
-        <v>-3.9</v>
+        <v>-5.2</v>
       </c>
       <c r="C82">
         <v>81</v>
@@ -1671,10 +1682,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B83">
-        <v>-4.0999999999999996</v>
+        <v>-5.5</v>
       </c>
       <c r="C83">
         <v>82</v>
@@ -1682,10 +1693,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B84">
-        <v>-4.0999999999999996</v>
+        <v>-5.7</v>
       </c>
       <c r="C84">
         <v>83</v>
@@ -1693,10 +1704,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B85">
-        <v>-4.8</v>
+        <v>-5.9</v>
       </c>
       <c r="C85">
         <v>84</v>
@@ -1704,10 +1715,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B86">
-        <v>-5.3</v>
+        <v>-6.2</v>
       </c>
       <c r="C86">
         <v>85</v>
@@ -1718,7 +1729,7 @@
         <v>83</v>
       </c>
       <c r="B87">
-        <v>-5.8</v>
+        <v>-6.4</v>
       </c>
       <c r="C87">
         <v>86</v>
@@ -1726,10 +1737,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="B88">
-        <v>-5.8</v>
+        <v>-6.6</v>
       </c>
       <c r="C88">
         <v>87</v>
@@ -1737,10 +1748,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B89">
-        <v>-6.7</v>
+        <v>-6.8</v>
       </c>
       <c r="C89">
         <v>88</v>
@@ -1748,10 +1759,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B90">
-        <v>-6.7</v>
+        <v>-6.9</v>
       </c>
       <c r="C90">
         <v>89</v>
@@ -1759,10 +1770,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B91">
-        <v>-7.3</v>
+        <v>-7</v>
       </c>
       <c r="C91">
         <v>90</v>
@@ -1770,10 +1781,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B92">
-        <v>-7.7</v>
+        <v>-7.5</v>
       </c>
       <c r="C92">
         <v>91</v>
@@ -1781,10 +1792,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B93">
-        <v>-8</v>
+        <v>-7.6</v>
       </c>
       <c r="C93">
         <v>92</v>
@@ -1792,10 +1803,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B94">
-        <v>-8.1999999999999993</v>
+        <v>-7.7</v>
       </c>
       <c r="C94">
         <v>93</v>
@@ -1803,10 +1814,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B95">
-        <v>-8.1999999999999993</v>
+        <v>-7.8</v>
       </c>
       <c r="C95">
         <v>94</v>
@@ -1814,10 +1825,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B96">
-        <v>-8.3000000000000007</v>
+        <v>-7.9</v>
       </c>
       <c r="C96">
         <v>95</v>
@@ -1828,7 +1839,7 @@
         <v>105</v>
       </c>
       <c r="B97">
-        <v>-8.8000000000000007</v>
+        <v>-7.9</v>
       </c>
       <c r="C97">
         <v>96</v>
@@ -1836,10 +1847,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B98">
-        <v>-9.1</v>
+        <v>-8</v>
       </c>
       <c r="C98">
         <v>97</v>
@@ -1847,10 +1858,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B99">
-        <v>-9.1999999999999993</v>
+        <v>-8.1</v>
       </c>
       <c r="C99">
         <v>98</v>
@@ -1858,10 +1869,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B100">
-        <v>-9.4</v>
+        <v>-8.5</v>
       </c>
       <c r="C100">
         <v>99</v>
@@ -1869,10 +1880,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B101">
-        <v>-9.6</v>
+        <v>-8.5</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -1880,10 +1891,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B102">
-        <v>-9.8000000000000007</v>
+        <v>-8.5</v>
       </c>
       <c r="C102">
         <v>101</v>
@@ -1894,7 +1905,7 @@
         <v>104</v>
       </c>
       <c r="B103">
-        <v>-10</v>
+        <v>-9.4</v>
       </c>
       <c r="C103">
         <v>102</v>
@@ -1902,10 +1913,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B104">
-        <v>-10.6</v>
+        <v>-9.6</v>
       </c>
       <c r="C104">
         <v>103</v>
@@ -1913,10 +1924,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B105">
-        <v>-10.8</v>
+        <v>-9.6</v>
       </c>
       <c r="C105">
         <v>104</v>
@@ -1924,10 +1935,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B106">
-        <v>-10.8</v>
+        <v>-9.8000000000000007</v>
       </c>
       <c r="C106">
         <v>105</v>
@@ -1935,10 +1946,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B107">
-        <v>-10.8</v>
+        <v>-9.9</v>
       </c>
       <c r="C107">
         <v>106</v>
@@ -1946,10 +1957,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B108">
-        <v>-10.9</v>
+        <v>-10.4</v>
       </c>
       <c r="C108">
         <v>107</v>
@@ -1957,10 +1968,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B109">
-        <v>-11.6</v>
+        <v>-10.6</v>
       </c>
       <c r="C109">
         <v>108</v>
@@ -1968,10 +1979,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B110">
-        <v>-11.8</v>
+        <v>-11.5</v>
       </c>
       <c r="C110">
         <v>109</v>
@@ -1979,10 +1990,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B111">
-        <v>-11.9</v>
+        <v>-11.6</v>
       </c>
       <c r="C111">
         <v>110</v>
@@ -1990,10 +2001,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B112">
-        <v>-12.3</v>
+        <v>-11.8</v>
       </c>
       <c r="C112">
         <v>111</v>
@@ -2001,10 +2012,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113">
-        <v>-13</v>
+        <v>-12.2</v>
       </c>
       <c r="C113">
         <v>112</v>
@@ -2012,10 +2023,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="B114">
-        <v>-13</v>
+        <v>-12.5</v>
       </c>
       <c r="C114">
         <v>113</v>
@@ -2023,10 +2034,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B115">
-        <v>-13</v>
+        <v>-12.8</v>
       </c>
       <c r="C115">
         <v>114</v>
@@ -2034,10 +2045,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B116">
-        <v>-13.4</v>
+        <v>-13.3</v>
       </c>
       <c r="C116">
         <v>115</v>
@@ -2045,10 +2056,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B117">
-        <v>-13.5</v>
+        <v>-13.4</v>
       </c>
       <c r="C117">
         <v>116</v>
@@ -2056,10 +2067,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B118">
-        <v>-15.2</v>
+        <v>-14.3</v>
       </c>
       <c r="C118">
         <v>117</v>
@@ -2067,10 +2078,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B119">
-        <v>-15.5</v>
+        <v>-15.8</v>
       </c>
       <c r="C119">
         <v>118</v>
@@ -2078,10 +2089,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B120">
-        <v>-15.5</v>
+        <v>-15.8</v>
       </c>
       <c r="C120">
         <v>119</v>
@@ -2089,10 +2100,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B121">
-        <v>-15.6</v>
+        <v>-16</v>
       </c>
       <c r="C121">
         <v>120</v>
@@ -2100,10 +2111,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B122">
-        <v>-15.9</v>
+        <v>-16.5</v>
       </c>
       <c r="C122">
         <v>121</v>
@@ -2111,10 +2122,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B123">
-        <v>-16</v>
+        <v>-16.600000000000001</v>
       </c>
       <c r="C123">
         <v>122</v>
@@ -2122,10 +2133,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B124">
-        <v>-16</v>
+        <v>-16.7</v>
       </c>
       <c r="C124">
         <v>123</v>
@@ -2133,10 +2144,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B125">
-        <v>-16.2</v>
+        <v>-17.5</v>
       </c>
       <c r="C125">
         <v>124</v>
@@ -2144,10 +2155,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B126">
-        <v>-16.8</v>
+        <v>-17.600000000000001</v>
       </c>
       <c r="C126">
         <v>125</v>
@@ -2155,10 +2166,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B127">
-        <v>-17.3</v>
+        <v>-18.399999999999999</v>
       </c>
       <c r="C127">
         <v>126</v>
@@ -2166,10 +2177,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B128">
-        <v>-17.399999999999999</v>
+        <v>-18.7</v>
       </c>
       <c r="C128">
         <v>127</v>
@@ -2177,10 +2188,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B129">
-        <v>-17.7</v>
+        <v>-19</v>
       </c>
       <c r="C129">
         <v>128</v>
@@ -2188,10 +2199,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B130">
-        <v>-17.899999999999999</v>
+        <v>-19.100000000000001</v>
       </c>
       <c r="C130">
         <v>129</v>
@@ -2199,10 +2210,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B131">
-        <v>-18.600000000000001</v>
+        <v>-20.6</v>
       </c>
       <c r="C131">
         <v>130</v>
@@ -2210,10 +2221,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B132">
-        <v>-20.5</v>
+        <v>-20.7</v>
       </c>
       <c r="C132">
         <v>131</v>
@@ -2221,10 +2232,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B133">
-        <v>-20.8</v>
+        <v>-21</v>
       </c>
       <c r="C133">
         <v>132</v>
@@ -2232,7 +2243,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B134">
         <v>-21</v>
@@ -2243,10 +2254,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B135">
-        <v>-22.1</v>
+        <v>-21.6</v>
       </c>
       <c r="C135">
         <v>134</v>
@@ -2254,10 +2265,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B136">
-        <v>-26.2</v>
+        <v>-22.3</v>
       </c>
       <c r="C136">
         <v>135</v>
@@ -2265,10 +2276,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B137">
-        <v>-26.3</v>
+        <v>-28.5</v>
       </c>
       <c r="C137">
         <v>136</v>

</xml_diff>

<commit_message>
Week 9 Data Update
</commit_message>
<xml_diff>
--- a/PEAR/kford.xlsx
+++ b/PEAR/kford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wpars\OneDrive\Documents\Post-School\Family Feud Data\PEAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCB4AF3-EC23-4EA8-B369-D53D17A077AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F5A40A-DA78-46B1-90E9-C6D01E9CF858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="G124" sqref="G124"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,7 +794,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>28.1</v>
+        <v>29.2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -805,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>24.2</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -813,10 +813,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>24.1</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -824,10 +824,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>23.7</v>
+        <v>25.4</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -835,10 +835,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -846,10 +846,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>22.1</v>
+        <v>22.4</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -857,10 +857,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>21.4</v>
+        <v>20.9</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -871,7 +871,7 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>21.1</v>
+        <v>20.6</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -879,10 +879,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>21.1</v>
+        <v>20.3</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>19.5</v>
+        <v>20.2</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -901,10 +901,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>18.8</v>
+        <v>19.3</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -912,10 +912,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>18.3</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B14">
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -934,10 +934,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>16.600000000000001</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>16.399999999999999</v>
+        <v>17.3</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -956,10 +956,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>15.6</v>
+        <v>16.2</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -967,10 +967,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>15.5</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -978,10 +978,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>15</v>
+        <v>15.9</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -992,7 +992,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>14.9</v>
+        <v>15.7</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1003,7 +1003,7 @@
         <v>11</v>
       </c>
       <c r="B21">
-        <v>14.8</v>
+        <v>14.9</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1011,10 +1011,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>13.9</v>
+        <v>14.4</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B23">
-        <v>13.5</v>
+        <v>13.4</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>13.4</v>
+        <v>13.2</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1047,7 +1047,7 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>13.4</v>
+        <v>12.8</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1055,10 +1055,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>13.2</v>
+        <v>12.8</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1066,10 +1066,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>13.1</v>
+        <v>12.8</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1077,10 +1077,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>12.8</v>
+        <v>12.3</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1099,10 +1099,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B30">
-        <v>11.4</v>
+        <v>11.6</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B31">
-        <v>10.199999999999999</v>
+        <v>11</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>10.1</v>
+        <v>10.3</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1132,10 +1132,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B33">
-        <v>10</v>
+        <v>10.3</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B34">
-        <v>9.9</v>
+        <v>10</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B35">
-        <v>9.6999999999999993</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1165,10 +1165,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B36">
-        <v>9.4</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1176,10 +1176,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B37">
-        <v>9.1</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1187,10 +1187,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B38">
-        <v>8.9</v>
+        <v>9.6</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B39">
-        <v>8.6</v>
+        <v>9.4</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1209,10 +1209,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B40">
-        <v>8.4</v>
+        <v>9.1</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1220,10 +1220,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B41">
-        <v>8.4</v>
+        <v>9.1</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42">
-        <v>8.3000000000000007</v>
+        <v>8.4</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1245,7 +1245,7 @@
         <v>39</v>
       </c>
       <c r="B43">
-        <v>8.1999999999999993</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1256,7 +1256,7 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>8.1999999999999993</v>
+        <v>7.8</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1264,10 +1264,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
-        <v>7.7</v>
+        <v>7.8</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B46">
         <v>7.6</v>
@@ -1286,10 +1286,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B47">
-        <v>7.6</v>
+        <v>7.4</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B48">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -1308,10 +1308,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49">
-        <v>6.2</v>
+        <v>5.8</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -1319,10 +1319,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B50">
-        <v>5.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -1330,10 +1330,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B51">
-        <v>4.5999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -1341,10 +1341,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B52">
-        <v>4.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C52">
         <v>51</v>
@@ -1352,10 +1352,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B53">
-        <v>4.0999999999999996</v>
+        <v>5</v>
       </c>
       <c r="C53">
         <v>52</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -1374,10 +1374,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="C55">
         <v>54</v>
@@ -1385,10 +1385,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B56">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="C56">
         <v>55</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B57">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="C57">
         <v>56</v>
@@ -1407,10 +1407,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B58">
-        <v>3.2</v>
+        <v>3.7</v>
       </c>
       <c r="C58">
         <v>57</v>
@@ -1418,10 +1418,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -1429,10 +1429,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B60">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="C60">
         <v>59</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B61">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B62">
-        <v>2.2999999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="C62">
         <v>61</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B63">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -1476,7 +1476,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -1484,10 +1484,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B65">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
       <c r="C65">
         <v>64</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B66">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C66">
         <v>65</v>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B67">
-        <v>0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="C67">
         <v>66</v>
@@ -1517,10 +1517,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B68">
-        <v>0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="C68">
         <v>67</v>
@@ -1528,10 +1528,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -1539,10 +1539,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B70">
-        <v>-0.7</v>
+        <v>-1.5</v>
       </c>
       <c r="C70">
         <v>69</v>
@@ -1550,10 +1550,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B71">
-        <v>-0.7</v>
+        <v>-1.6</v>
       </c>
       <c r="C71">
         <v>70</v>
@@ -1561,10 +1561,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B72">
-        <v>-0.9</v>
+        <v>-1.7</v>
       </c>
       <c r="C72">
         <v>71</v>
@@ -1575,7 +1575,7 @@
         <v>69</v>
       </c>
       <c r="B73">
-        <v>-1</v>
+        <v>-1.9</v>
       </c>
       <c r="C73">
         <v>72</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B74">
-        <v>-1</v>
+        <v>-2.1</v>
       </c>
       <c r="C74">
         <v>73</v>
@@ -1594,10 +1594,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B75">
-        <v>-2.2000000000000002</v>
+        <v>-2.6</v>
       </c>
       <c r="C75">
         <v>74</v>
@@ -1605,10 +1605,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B76">
-        <v>-2.7</v>
+        <v>-3.2</v>
       </c>
       <c r="C76">
         <v>75</v>
@@ -1616,10 +1616,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>-3</v>
+        <v>-3.2</v>
       </c>
       <c r="C77">
         <v>76</v>
@@ -1627,10 +1627,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B78">
-        <v>-3.2</v>
+        <v>-3.4</v>
       </c>
       <c r="C78">
         <v>77</v>
@@ -1641,7 +1641,7 @@
         <v>73</v>
       </c>
       <c r="B79">
-        <v>-3.7</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="C79">
         <v>78</v>
@@ -1649,10 +1649,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B80">
-        <v>-3.9</v>
+        <v>-4.3</v>
       </c>
       <c r="C80">
         <v>79</v>
@@ -1660,10 +1660,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B81">
-        <v>-4.0999999999999996</v>
+        <v>-4.3</v>
       </c>
       <c r="C81">
         <v>80</v>
@@ -1671,10 +1671,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B82">
-        <v>-5.2</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="C82">
         <v>81</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B83">
-        <v>-5.5</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="C83">
         <v>82</v>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B84">
-        <v>-5.7</v>
+        <v>-5.5</v>
       </c>
       <c r="C84">
         <v>83</v>
@@ -1704,10 +1704,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B85">
-        <v>-5.9</v>
+        <v>-5.6</v>
       </c>
       <c r="C85">
         <v>84</v>
@@ -1715,10 +1715,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B86">
-        <v>-6.2</v>
+        <v>-5.8</v>
       </c>
       <c r="C86">
         <v>85</v>
@@ -1726,10 +1726,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="B87">
-        <v>-6.4</v>
+        <v>-5.9</v>
       </c>
       <c r="C87">
         <v>86</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B88">
-        <v>-6.6</v>
+        <v>-6</v>
       </c>
       <c r="C88">
         <v>87</v>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B89">
-        <v>-6.8</v>
+        <v>-6.3</v>
       </c>
       <c r="C89">
         <v>88</v>
@@ -1759,10 +1759,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B90">
-        <v>-6.9</v>
+        <v>-6.6</v>
       </c>
       <c r="C90">
         <v>89</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B91">
-        <v>-7</v>
+        <v>-6.6</v>
       </c>
       <c r="C91">
         <v>90</v>
@@ -1781,10 +1781,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B92">
-        <v>-7.5</v>
+        <v>-6.9</v>
       </c>
       <c r="C92">
         <v>91</v>
@@ -1792,10 +1792,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B93">
-        <v>-7.6</v>
+        <v>-7.2</v>
       </c>
       <c r="C93">
         <v>92</v>
@@ -1803,10 +1803,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B94">
-        <v>-7.7</v>
+        <v>-7.5</v>
       </c>
       <c r="C94">
         <v>93</v>
@@ -1814,10 +1814,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B95">
-        <v>-7.8</v>
+        <v>-7.9</v>
       </c>
       <c r="C95">
         <v>94</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B96">
-        <v>-7.9</v>
+        <v>-8.4</v>
       </c>
       <c r="C96">
         <v>95</v>
@@ -1836,10 +1836,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B97">
-        <v>-7.9</v>
+        <v>-8.6</v>
       </c>
       <c r="C97">
         <v>96</v>
@@ -1847,10 +1847,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="B98">
-        <v>-8</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="C98">
         <v>97</v>
@@ -1858,10 +1858,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B99">
-        <v>-8.1</v>
+        <v>-9</v>
       </c>
       <c r="C99">
         <v>98</v>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B100">
-        <v>-8.5</v>
+        <v>-9.1999999999999993</v>
       </c>
       <c r="C100">
         <v>99</v>
@@ -1880,10 +1880,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="B101">
-        <v>-8.5</v>
+        <v>-9.6</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -1891,10 +1891,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B102">
-        <v>-8.5</v>
+        <v>-10.1</v>
       </c>
       <c r="C102">
         <v>101</v>
@@ -1902,10 +1902,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B103">
-        <v>-9.4</v>
+        <v>-10.1</v>
       </c>
       <c r="C103">
         <v>102</v>
@@ -1913,10 +1913,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B104">
-        <v>-9.6</v>
+        <v>-10.3</v>
       </c>
       <c r="C104">
         <v>103</v>
@@ -1924,10 +1924,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B105">
-        <v>-9.6</v>
+        <v>-10.4</v>
       </c>
       <c r="C105">
         <v>104</v>
@@ -1935,10 +1935,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B106">
-        <v>-9.8000000000000007</v>
+        <v>-10.5</v>
       </c>
       <c r="C106">
         <v>105</v>
@@ -1946,10 +1946,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B107">
-        <v>-9.9</v>
+        <v>-11.1</v>
       </c>
       <c r="C107">
         <v>106</v>
@@ -1957,10 +1957,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B108">
-        <v>-10.4</v>
+        <v>-11.3</v>
       </c>
       <c r="C108">
         <v>107</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B109">
-        <v>-10.6</v>
+        <v>-11.5</v>
       </c>
       <c r="C109">
         <v>108</v>
@@ -1979,10 +1979,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B110">
-        <v>-11.5</v>
+        <v>-11.6</v>
       </c>
       <c r="C110">
         <v>109</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B111">
         <v>-11.6</v>
@@ -2001,10 +2001,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B112">
-        <v>-11.8</v>
+        <v>-12.1</v>
       </c>
       <c r="C112">
         <v>111</v>
@@ -2012,10 +2012,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B113">
-        <v>-12.2</v>
+        <v>-12.6</v>
       </c>
       <c r="C113">
         <v>112</v>
@@ -2023,10 +2023,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B114">
-        <v>-12.5</v>
+        <v>-12.6</v>
       </c>
       <c r="C114">
         <v>113</v>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B115">
-        <v>-12.8</v>
+        <v>-12.9</v>
       </c>
       <c r="C115">
         <v>114</v>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B116">
-        <v>-13.3</v>
+        <v>-14.1</v>
       </c>
       <c r="C116">
         <v>115</v>
@@ -2056,10 +2056,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B117">
-        <v>-13.4</v>
+        <v>-14.6</v>
       </c>
       <c r="C117">
         <v>116</v>
@@ -2070,7 +2070,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>-14.3</v>
+        <v>-15.1</v>
       </c>
       <c r="C118">
         <v>117</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B119">
-        <v>-15.8</v>
+        <v>-15.3</v>
       </c>
       <c r="C119">
         <v>118</v>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B120">
-        <v>-15.8</v>
+        <v>-15.3</v>
       </c>
       <c r="C120">
         <v>119</v>
@@ -2100,10 +2100,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B121">
-        <v>-16</v>
+        <v>-15.6</v>
       </c>
       <c r="C121">
         <v>120</v>
@@ -2111,10 +2111,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B122">
-        <v>-16.5</v>
+        <v>-15.9</v>
       </c>
       <c r="C122">
         <v>121</v>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B123">
-        <v>-16.600000000000001</v>
+        <v>-16.2</v>
       </c>
       <c r="C123">
         <v>122</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B124">
         <v>-16.7</v>
@@ -2144,10 +2144,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B125">
-        <v>-17.5</v>
+        <v>-17</v>
       </c>
       <c r="C125">
         <v>124</v>
@@ -2155,10 +2155,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B126">
-        <v>-17.600000000000001</v>
+        <v>-17.3</v>
       </c>
       <c r="C126">
         <v>125</v>
@@ -2166,10 +2166,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B127">
-        <v>-18.399999999999999</v>
+        <v>-17.7</v>
       </c>
       <c r="C127">
         <v>126</v>
@@ -2177,10 +2177,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B128">
-        <v>-18.7</v>
+        <v>-18.3</v>
       </c>
       <c r="C128">
         <v>127</v>
@@ -2188,10 +2188,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B129">
-        <v>-19</v>
+        <v>-18.8</v>
       </c>
       <c r="C129">
         <v>128</v>
@@ -2199,10 +2199,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B130">
-        <v>-19.100000000000001</v>
+        <v>-19.600000000000001</v>
       </c>
       <c r="C130">
         <v>129</v>
@@ -2210,10 +2210,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B131">
-        <v>-20.6</v>
+        <v>-20.3</v>
       </c>
       <c r="C131">
         <v>130</v>
@@ -2224,7 +2224,7 @@
         <v>133</v>
       </c>
       <c r="B132">
-        <v>-20.7</v>
+        <v>-22.9</v>
       </c>
       <c r="C132">
         <v>131</v>
@@ -2235,7 +2235,7 @@
         <v>134</v>
       </c>
       <c r="B133">
-        <v>-21</v>
+        <v>-22.9</v>
       </c>
       <c r="C133">
         <v>132</v>
@@ -2246,7 +2246,7 @@
         <v>129</v>
       </c>
       <c r="B134">
-        <v>-21</v>
+        <v>-23.2</v>
       </c>
       <c r="C134">
         <v>133</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B135">
-        <v>-21.6</v>
+        <v>-23.5</v>
       </c>
       <c r="C135">
         <v>134</v>
@@ -2265,10 +2265,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B136">
-        <v>-22.3</v>
+        <v>-24.5</v>
       </c>
       <c r="C136">
         <v>135</v>
@@ -2279,7 +2279,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>-28.5</v>
+        <v>-27.2</v>
       </c>
       <c r="C137">
         <v>136</v>

</xml_diff>

<commit_message>
Week 10 Data Update
</commit_message>
<xml_diff>
--- a/PEAR/kford.xlsx
+++ b/PEAR/kford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wpars\OneDrive\Documents\Post-School\Family Feud Data\PEAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F5A40A-DA78-46B1-90E9-C6D01E9CF858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E497ABD-FA3B-43EE-B7A0-61A7D39E8DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -772,11 +772,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -794,7 +797,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>29.2</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -805,7 +808,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>26</v>
+        <v>27.9</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -813,10 +816,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>26</v>
+        <v>25.3</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -824,10 +827,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>25.4</v>
+        <v>25.1</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -838,7 +841,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>24.5</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -860,7 +863,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>20.9</v>
+        <v>21.1</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -868,10 +871,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>20.6</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -879,10 +882,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B10">
-        <v>20.3</v>
+        <v>20.7</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -890,10 +893,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>20.2</v>
+        <v>20.6</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -901,10 +904,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12">
-        <v>19.3</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -912,10 +915,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>18.600000000000001</v>
+        <v>19.8</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -923,10 +926,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>18.5</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -934,10 +937,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>17.399999999999999</v>
+        <v>17.5</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -945,7 +948,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>17.3</v>
@@ -956,10 +959,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>16.2</v>
+        <v>16.8</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -967,10 +970,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>16.100000000000001</v>
+        <v>15.6</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -978,10 +981,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>15.9</v>
+        <v>15.5</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -989,10 +992,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B20">
-        <v>15.7</v>
+        <v>15.4</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1000,10 +1003,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>14.9</v>
+        <v>15.3</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1011,10 +1014,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>14.4</v>
+        <v>14.8</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1022,10 +1025,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>13.4</v>
+        <v>14.1</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1033,10 +1036,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B24">
-        <v>13.2</v>
+        <v>13.9</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1044,10 +1047,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>12.8</v>
+        <v>13.5</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1055,10 +1058,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B26">
-        <v>12.8</v>
+        <v>12.3</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1066,10 +1069,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>12.8</v>
+        <v>12.2</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1077,10 +1080,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B28">
-        <v>12.3</v>
+        <v>11.7</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1088,10 +1091,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B29">
-        <v>12.1</v>
+        <v>11.7</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1099,10 +1102,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>11.6</v>
+        <v>11.7</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1110,10 +1113,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B31">
-        <v>11</v>
+        <v>11.1</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1121,10 +1124,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B32">
-        <v>10.3</v>
+        <v>11</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1132,10 +1135,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B33">
-        <v>10.3</v>
+        <v>9.9</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1143,10 +1146,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B34">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -1154,10 +1157,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B35">
-        <v>9.8000000000000007</v>
+        <v>9.9</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1165,10 +1168,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B36">
-        <v>9.6999999999999993</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1176,10 +1179,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B37">
-        <v>9.6999999999999993</v>
+        <v>9.6</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1187,10 +1190,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B38">
-        <v>9.6</v>
+        <v>9.5</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1198,10 +1201,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B39">
-        <v>9.4</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1209,10 +1212,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B40">
-        <v>9.1</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1220,10 +1223,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B41">
-        <v>9.1</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1231,10 +1234,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B42">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1242,10 +1245,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B43">
-        <v>8.3000000000000007</v>
+        <v>7.9</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1253,10 +1256,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B44">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1267,7 +1270,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>7.8</v>
+        <v>7.5</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1275,10 +1278,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B46">
-        <v>7.6</v>
+        <v>7</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -1286,10 +1289,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B47">
-        <v>7.4</v>
+        <v>6.7</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1297,10 +1300,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B48">
-        <v>7</v>
+        <v>6.3</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -1308,7 +1311,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B49">
         <v>5.8</v>
@@ -1319,10 +1322,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B50">
-        <v>8.1999999999999993</v>
+        <v>5.8</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -1330,10 +1333,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B51">
-        <v>8.1</v>
+        <v>5.7</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -1341,10 +1344,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B52">
-        <v>5.0999999999999996</v>
+        <v>5.3</v>
       </c>
       <c r="C52">
         <v>51</v>
@@ -1352,10 +1355,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="C53">
         <v>52</v>
@@ -1363,10 +1366,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="C54">
         <v>53</v>
@@ -1374,10 +1377,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B55">
-        <v>3.9</v>
+        <v>3.6</v>
       </c>
       <c r="C55">
         <v>54</v>
@@ -1385,10 +1388,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B56">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="C56">
         <v>55</v>
@@ -1396,10 +1399,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B57">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="C57">
         <v>56</v>
@@ -1407,10 +1410,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B58">
-        <v>3.7</v>
+        <v>3.2</v>
       </c>
       <c r="C58">
         <v>57</v>
@@ -1418,10 +1421,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B59">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -1429,10 +1432,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B60">
-        <v>3.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C60">
         <v>59</v>
@@ -1440,10 +1443,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -1451,10 +1454,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B62">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="C62">
         <v>61</v>
@@ -1462,10 +1465,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B63">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -1473,10 +1476,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B64">
-        <v>1.7</v>
+        <v>1.2</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -1484,10 +1487,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B65">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C65">
         <v>64</v>
@@ -1495,7 +1498,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B66">
         <v>0.4</v>
@@ -1506,7 +1509,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B67">
         <v>-0.2</v>
@@ -1517,10 +1520,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B68">
-        <v>-0.3</v>
+        <v>-0.5</v>
       </c>
       <c r="C68">
         <v>67</v>
@@ -1528,10 +1531,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B69">
-        <v>-0.5</v>
+        <v>-0.6</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -1539,10 +1542,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B70">
-        <v>-1.5</v>
+        <v>-0.8</v>
       </c>
       <c r="C70">
         <v>69</v>
@@ -1550,10 +1553,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B71">
-        <v>-1.6</v>
+        <v>-1.7</v>
       </c>
       <c r="C71">
         <v>70</v>
@@ -1561,10 +1564,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="B72">
-        <v>-1.7</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="C72">
         <v>71</v>
@@ -1572,10 +1575,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B73">
-        <v>-1.9</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="C73">
         <v>72</v>
@@ -1583,10 +1586,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B74">
-        <v>-2.1</v>
+        <v>-2.5</v>
       </c>
       <c r="C74">
         <v>73</v>
@@ -1594,10 +1597,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B75">
-        <v>-2.6</v>
+        <v>-2.8</v>
       </c>
       <c r="C75">
         <v>74</v>
@@ -1605,10 +1608,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B76">
-        <v>-3.2</v>
+        <v>-3.1</v>
       </c>
       <c r="C76">
         <v>75</v>
@@ -1616,7 +1619,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B77">
         <v>-3.2</v>
@@ -1627,7 +1630,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B78">
         <v>-3.4</v>
@@ -1638,10 +1641,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B79">
-        <v>-4.0999999999999996</v>
+        <v>-3.6</v>
       </c>
       <c r="C79">
         <v>78</v>
@@ -1652,7 +1655,7 @@
         <v>89</v>
       </c>
       <c r="B80">
-        <v>-4.3</v>
+        <v>-3.7</v>
       </c>
       <c r="C80">
         <v>79</v>
@@ -1660,10 +1663,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B81">
-        <v>-4.3</v>
+        <v>-4</v>
       </c>
       <c r="C81">
         <v>80</v>
@@ -1674,7 +1677,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>-4.5999999999999996</v>
+        <v>-4.2</v>
       </c>
       <c r="C82">
         <v>81</v>
@@ -1682,10 +1685,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="B83">
-        <v>-4.5999999999999996</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="C83">
         <v>82</v>
@@ -1693,10 +1696,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B84">
-        <v>-5.5</v>
+        <v>-5</v>
       </c>
       <c r="C84">
         <v>83</v>
@@ -1704,10 +1707,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B85">
-        <v>-5.6</v>
+        <v>-5.7</v>
       </c>
       <c r="C85">
         <v>84</v>
@@ -1715,10 +1718,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B86">
-        <v>-5.8</v>
+        <v>-5.7</v>
       </c>
       <c r="C86">
         <v>85</v>
@@ -1726,10 +1729,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B87">
-        <v>-5.9</v>
+        <v>-6</v>
       </c>
       <c r="C87">
         <v>86</v>
@@ -1737,10 +1740,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B88">
-        <v>-6</v>
+        <v>-6.3</v>
       </c>
       <c r="C88">
         <v>87</v>
@@ -1748,10 +1751,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B89">
-        <v>-6.3</v>
+        <v>-6.6</v>
       </c>
       <c r="C89">
         <v>88</v>
@@ -1759,10 +1762,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B90">
-        <v>-6.6</v>
+        <v>-7</v>
       </c>
       <c r="C90">
         <v>89</v>
@@ -1770,10 +1773,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B91">
-        <v>-6.6</v>
+        <v>-7.3</v>
       </c>
       <c r="C91">
         <v>90</v>
@@ -1781,10 +1784,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B92">
-        <v>-6.9</v>
+        <v>-7.4</v>
       </c>
       <c r="C92">
         <v>91</v>
@@ -1792,10 +1795,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B93">
-        <v>-7.2</v>
+        <v>-7.4</v>
       </c>
       <c r="C93">
         <v>92</v>
@@ -1803,7 +1806,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="B94">
         <v>-7.5</v>
@@ -1814,10 +1817,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="B95">
-        <v>-7.9</v>
+        <v>-7.6</v>
       </c>
       <c r="C95">
         <v>94</v>
@@ -1825,10 +1828,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B96">
-        <v>-8.4</v>
+        <v>-7.8</v>
       </c>
       <c r="C96">
         <v>95</v>
@@ -1836,10 +1839,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B97">
-        <v>-8.6</v>
+        <v>-8.1</v>
       </c>
       <c r="C97">
         <v>96</v>
@@ -1847,10 +1850,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="B98">
-        <v>-8.8000000000000007</v>
+        <v>-8.1</v>
       </c>
       <c r="C98">
         <v>97</v>
@@ -1858,10 +1861,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B99">
-        <v>-9</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="C99">
         <v>98</v>
@@ -1869,10 +1872,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B100">
-        <v>-9.1999999999999993</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="C100">
         <v>99</v>
@@ -1880,10 +1883,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="B101">
-        <v>-9.6</v>
+        <v>-9.1999999999999993</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -1894,7 +1897,7 @@
         <v>99</v>
       </c>
       <c r="B102">
-        <v>-10.1</v>
+        <v>-9.9</v>
       </c>
       <c r="C102">
         <v>101</v>
@@ -1902,10 +1905,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B103">
-        <v>-10.1</v>
+        <v>-10.199999999999999</v>
       </c>
       <c r="C103">
         <v>102</v>
@@ -1913,10 +1916,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B104">
-        <v>-10.3</v>
+        <v>-10.4</v>
       </c>
       <c r="C104">
         <v>103</v>
@@ -1924,10 +1927,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B105">
-        <v>-10.4</v>
+        <v>-10.9</v>
       </c>
       <c r="C105">
         <v>104</v>
@@ -1935,10 +1938,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B106">
-        <v>-10.5</v>
+        <v>-10.9</v>
       </c>
       <c r="C106">
         <v>105</v>
@@ -1946,10 +1949,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B107">
-        <v>-11.1</v>
+        <v>-11.2</v>
       </c>
       <c r="C107">
         <v>106</v>
@@ -1957,10 +1960,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B108">
-        <v>-11.3</v>
+        <v>-11.7</v>
       </c>
       <c r="C108">
         <v>107</v>
@@ -1968,10 +1971,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="B109">
-        <v>-11.5</v>
+        <v>-11.8</v>
       </c>
       <c r="C109">
         <v>108</v>
@@ -1979,10 +1982,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B110">
-        <v>-11.6</v>
+        <v>-11.8</v>
       </c>
       <c r="C110">
         <v>109</v>
@@ -1990,10 +1993,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B111">
-        <v>-11.6</v>
+        <v>-12.2</v>
       </c>
       <c r="C111">
         <v>110</v>
@@ -2001,10 +2004,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B112">
-        <v>-12.1</v>
+        <v>-12.3</v>
       </c>
       <c r="C112">
         <v>111</v>
@@ -2023,10 +2026,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B114">
-        <v>-12.6</v>
+        <v>-12.9</v>
       </c>
       <c r="C114">
         <v>113</v>
@@ -2034,10 +2037,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B115">
-        <v>-12.9</v>
+        <v>-13.4</v>
       </c>
       <c r="C115">
         <v>114</v>
@@ -2045,10 +2048,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="B116">
-        <v>-14.1</v>
+        <v>-13.6</v>
       </c>
       <c r="C116">
         <v>115</v>
@@ -2056,10 +2059,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B117">
-        <v>-14.6</v>
+        <v>-14.4</v>
       </c>
       <c r="C117">
         <v>116</v>
@@ -2067,10 +2070,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B118">
-        <v>-15.1</v>
+        <v>-14.6</v>
       </c>
       <c r="C118">
         <v>117</v>
@@ -2078,10 +2081,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B119">
-        <v>-15.3</v>
+        <v>-15.1</v>
       </c>
       <c r="C119">
         <v>118</v>
@@ -2089,10 +2092,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B120">
-        <v>-15.3</v>
+        <v>-15.2</v>
       </c>
       <c r="C120">
         <v>119</v>
@@ -2100,10 +2103,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B121">
-        <v>-15.6</v>
+        <v>-15.3</v>
       </c>
       <c r="C121">
         <v>120</v>
@@ -2111,10 +2114,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B122">
-        <v>-15.9</v>
+        <v>-16</v>
       </c>
       <c r="C122">
         <v>121</v>
@@ -2122,10 +2125,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B123">
-        <v>-16.2</v>
+        <v>-16.100000000000001</v>
       </c>
       <c r="C123">
         <v>122</v>
@@ -2133,10 +2136,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B124">
-        <v>-16.7</v>
+        <v>-16.2</v>
       </c>
       <c r="C124">
         <v>123</v>
@@ -2144,10 +2147,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B125">
-        <v>-17</v>
+        <v>-16.8</v>
       </c>
       <c r="C125">
         <v>124</v>
@@ -2155,10 +2158,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B126">
-        <v>-17.3</v>
+        <v>-16.899999999999999</v>
       </c>
       <c r="C126">
         <v>125</v>
@@ -2166,10 +2169,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B127">
-        <v>-17.7</v>
+        <v>-17.899999999999999</v>
       </c>
       <c r="C127">
         <v>126</v>
@@ -2177,10 +2180,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B128">
-        <v>-18.3</v>
+        <v>-18.2</v>
       </c>
       <c r="C128">
         <v>127</v>
@@ -2188,10 +2191,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B129">
-        <v>-18.8</v>
+        <v>-19.100000000000001</v>
       </c>
       <c r="C129">
         <v>128</v>
@@ -2199,10 +2202,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B130">
-        <v>-19.600000000000001</v>
+        <v>-19.8</v>
       </c>
       <c r="C130">
         <v>129</v>
@@ -2213,7 +2216,7 @@
         <v>128</v>
       </c>
       <c r="B131">
-        <v>-20.3</v>
+        <v>-20</v>
       </c>
       <c r="C131">
         <v>130</v>
@@ -2221,10 +2224,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B132">
-        <v>-22.9</v>
+        <v>-20.100000000000001</v>
       </c>
       <c r="C132">
         <v>131</v>
@@ -2235,7 +2238,7 @@
         <v>134</v>
       </c>
       <c r="B133">
-        <v>-22.9</v>
+        <v>-21</v>
       </c>
       <c r="C133">
         <v>132</v>
@@ -2243,10 +2246,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B134">
-        <v>-23.2</v>
+        <v>-23.1</v>
       </c>
       <c r="C134">
         <v>133</v>
@@ -2254,10 +2257,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B135">
-        <v>-23.5</v>
+        <v>-23.4</v>
       </c>
       <c r="C135">
         <v>134</v>
@@ -2268,7 +2271,7 @@
         <v>132</v>
       </c>
       <c r="B136">
-        <v>-24.5</v>
+        <v>-24.3</v>
       </c>
       <c r="C136">
         <v>135</v>
@@ -2279,7 +2282,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>-27.2</v>
+        <v>-28</v>
       </c>
       <c r="C137">
         <v>136</v>

</xml_diff>

<commit_message>
Week 11 Data Update
</commit_message>
<xml_diff>
--- a/PEAR/kford.xlsx
+++ b/PEAR/kford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wpars\OneDrive\Documents\Post-School\Family Feud Data\PEAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E497ABD-FA3B-43EE-B7A0-61A7D39E8DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3C64AF-44FD-46A7-8EB2-55946BA2D542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,10 +794,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>29</v>
+        <v>29.8</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -805,10 +805,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>27.9</v>
+        <v>29.6</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>25.3</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>25.1</v>
+        <v>23.8</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -838,10 +838,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>24</v>
+        <v>23.8</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -849,10 +849,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>22.4</v>
+        <v>21.8</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -860,10 +860,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>21.1</v>
+        <v>21.6</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -871,10 +871,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>21.6</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -882,10 +882,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>20.7</v>
+        <v>20.9</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -893,10 +893,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>20.6</v>
+        <v>19.8</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -904,10 +904,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>19.8</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -918,7 +918,7 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>19.8</v>
+        <v>19.5</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -948,10 +948,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B16">
-        <v>17.3</v>
+        <v>15.9</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -959,10 +959,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>16.8</v>
+        <v>15.9</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -970,10 +970,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B18">
-        <v>15.6</v>
+        <v>15.9</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -981,10 +981,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>15.5</v>
+        <v>15.9</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -995,7 +995,7 @@
         <v>32</v>
       </c>
       <c r="B20">
-        <v>15.4</v>
+        <v>15.3</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1006,7 +1006,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>15.3</v>
+        <v>15.2</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1014,10 +1014,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>14.8</v>
+        <v>14.3</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B23">
         <v>14.1</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24">
-        <v>13.9</v>
+        <v>13.7</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B25">
-        <v>13.5</v>
+        <v>13.6</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>12.3</v>
+        <v>12.6</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1069,10 +1069,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27">
-        <v>12.2</v>
+        <v>12.4</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1080,10 +1080,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B28">
-        <v>11.7</v>
+        <v>12.1</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1091,10 +1091,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B29">
-        <v>11.7</v>
+        <v>11.9</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B30">
-        <v>11.7</v>
+        <v>10.8</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1113,10 +1113,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B31">
-        <v>11.1</v>
+        <v>10.4</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1124,10 +1124,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>10.1</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B33">
-        <v>9.9</v>
+        <v>9.6</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1146,10 +1146,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B34">
-        <v>9.9</v>
+        <v>9.6</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B35">
-        <v>9.9</v>
+        <v>9.5</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1171,7 +1171,7 @@
         <v>42</v>
       </c>
       <c r="B36">
-        <v>9.8000000000000007</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1182,7 +1182,7 @@
         <v>48</v>
       </c>
       <c r="B37">
-        <v>9.6</v>
+        <v>8.9</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1190,10 +1190,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B38">
-        <v>9.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1201,10 +1201,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B39">
-        <v>9.1999999999999993</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B40">
-        <v>8.8000000000000007</v>
+        <v>8.6</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B41">
-        <v>8.3000000000000007</v>
+        <v>8.6</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B42">
-        <v>8.1</v>
+        <v>8.5</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B43">
-        <v>7.9</v>
+        <v>8.4</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1256,10 +1256,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B44">
-        <v>7.6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B45">
-        <v>7.5</v>
+        <v>7.8</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1278,10 +1278,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B47">
-        <v>6.7</v>
+        <v>7.2</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B48">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -1311,10 +1311,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B49">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B51">
         <v>5.7</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B52">
-        <v>5.3</v>
+        <v>5</v>
       </c>
       <c r="C52">
         <v>51</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B53">
-        <v>5.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C53">
         <v>52</v>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B54">
-        <v>3.6</v>
+        <v>4.3</v>
       </c>
       <c r="C54">
         <v>53</v>
@@ -1377,10 +1377,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B55">
-        <v>3.6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C55">
         <v>54</v>
@@ -1388,10 +1388,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B56">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="C56">
         <v>55</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B57">
         <v>3.4</v>
@@ -1413,7 +1413,7 @@
         <v>78</v>
       </c>
       <c r="B58">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="C58">
         <v>57</v>
@@ -1421,10 +1421,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B59">
-        <v>3.1</v>
+        <v>1.8</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B60">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="C60">
         <v>59</v>
@@ -1443,10 +1443,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -1454,10 +1454,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B62">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="C62">
         <v>61</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B63">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -1479,7 +1479,7 @@
         <v>60</v>
       </c>
       <c r="B64">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -1487,10 +1487,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B65">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C65">
         <v>64</v>
@@ -1498,10 +1498,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B66">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="C66">
         <v>65</v>
@@ -1509,10 +1509,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B67">
-        <v>-0.2</v>
+        <v>-0.6</v>
       </c>
       <c r="C67">
         <v>66</v>
@@ -1520,10 +1520,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B68">
-        <v>-0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="C68">
         <v>67</v>
@@ -1531,10 +1531,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B69">
-        <v>-0.6</v>
+        <v>-0.8</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -1553,10 +1553,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B71">
-        <v>-1.7</v>
+        <v>-1.6</v>
       </c>
       <c r="C71">
         <v>70</v>
@@ -1564,10 +1564,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="B72">
-        <v>-2.2000000000000002</v>
+        <v>-1.8</v>
       </c>
       <c r="C72">
         <v>71</v>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B73">
-        <v>-2.2000000000000002</v>
+        <v>-1.9</v>
       </c>
       <c r="C73">
         <v>72</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B74">
-        <v>-2.5</v>
+        <v>-2.4</v>
       </c>
       <c r="C74">
         <v>73</v>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="B75">
-        <v>-2.8</v>
+        <v>-2.6</v>
       </c>
       <c r="C75">
         <v>74</v>
@@ -1608,10 +1608,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B76">
-        <v>-3.1</v>
+        <v>-2.9</v>
       </c>
       <c r="C76">
         <v>75</v>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>-3.2</v>
+        <v>-3.4</v>
       </c>
       <c r="C77">
         <v>76</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B78">
-        <v>-3.4</v>
+        <v>-3.6</v>
       </c>
       <c r="C78">
         <v>77</v>
@@ -1641,10 +1641,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B79">
-        <v>-3.6</v>
+        <v>-3.9</v>
       </c>
       <c r="C79">
         <v>78</v>
@@ -1652,10 +1652,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="B80">
-        <v>-3.7</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="C80">
         <v>79</v>
@@ -1663,10 +1663,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B81">
-        <v>-4</v>
+        <v>-4.5</v>
       </c>
       <c r="C81">
         <v>80</v>
@@ -1674,10 +1674,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B82">
-        <v>-4.2</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="C82">
         <v>81</v>
@@ -1685,10 +1685,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B83">
-        <v>-4.4000000000000004</v>
+        <v>-4.7</v>
       </c>
       <c r="C83">
         <v>82</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B84">
         <v>-5</v>
@@ -1710,7 +1710,7 @@
         <v>94</v>
       </c>
       <c r="B85">
-        <v>-5.7</v>
+        <v>-5.2</v>
       </c>
       <c r="C85">
         <v>84</v>
@@ -1718,10 +1718,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="B86">
-        <v>-5.7</v>
+        <v>-5.4</v>
       </c>
       <c r="C86">
         <v>85</v>
@@ -1732,7 +1732,7 @@
         <v>83</v>
       </c>
       <c r="B87">
-        <v>-6</v>
+        <v>-5.8</v>
       </c>
       <c r="C87">
         <v>86</v>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="B88">
-        <v>-6.3</v>
+        <v>-6.1</v>
       </c>
       <c r="C88">
         <v>87</v>
@@ -1751,10 +1751,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="B89">
-        <v>-6.6</v>
+        <v>-6.1</v>
       </c>
       <c r="C89">
         <v>88</v>
@@ -1762,10 +1762,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B90">
-        <v>-7</v>
+        <v>-6.3</v>
       </c>
       <c r="C90">
         <v>89</v>
@@ -1773,10 +1773,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="B91">
-        <v>-7.3</v>
+        <v>-7</v>
       </c>
       <c r="C91">
         <v>90</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B92">
-        <v>-7.4</v>
+        <v>-7.3</v>
       </c>
       <c r="C92">
         <v>91</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B93">
         <v>-7.4</v>
@@ -1806,10 +1806,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="B94">
-        <v>-7.5</v>
+        <v>-7.4</v>
       </c>
       <c r="C94">
         <v>93</v>
@@ -1817,10 +1817,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B95">
-        <v>-7.6</v>
+        <v>-7.9</v>
       </c>
       <c r="C95">
         <v>94</v>
@@ -1828,10 +1828,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B96">
-        <v>-7.8</v>
+        <v>-7.9</v>
       </c>
       <c r="C96">
         <v>95</v>
@@ -1839,10 +1839,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B97">
-        <v>-8.1</v>
+        <v>-8</v>
       </c>
       <c r="C97">
         <v>96</v>
@@ -1853,7 +1853,7 @@
         <v>103</v>
       </c>
       <c r="B98">
-        <v>-8.1</v>
+        <v>-8.3000000000000007</v>
       </c>
       <c r="C98">
         <v>97</v>
@@ -1861,10 +1861,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B99">
-        <v>-8.1999999999999993</v>
+        <v>-8.4</v>
       </c>
       <c r="C99">
         <v>98</v>
@@ -1872,10 +1872,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>-8.8000000000000007</v>
+        <v>-8.5</v>
       </c>
       <c r="C100">
         <v>99</v>
@@ -1883,10 +1883,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="B101">
-        <v>-9.1999999999999993</v>
+        <v>-9.3000000000000007</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -1894,10 +1894,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B102">
-        <v>-9.9</v>
+        <v>-9.4</v>
       </c>
       <c r="C102">
         <v>101</v>
@@ -1905,10 +1905,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B103">
-        <v>-10.199999999999999</v>
+        <v>-9.5</v>
       </c>
       <c r="C103">
         <v>102</v>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B104">
         <v>-10.4</v>
@@ -1927,10 +1927,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B105">
-        <v>-10.9</v>
+        <v>-10.7</v>
       </c>
       <c r="C105">
         <v>104</v>
@@ -1938,10 +1938,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="B106">
-        <v>-10.9</v>
+        <v>-10.7</v>
       </c>
       <c r="C106">
         <v>105</v>
@@ -1949,10 +1949,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B107">
-        <v>-11.2</v>
+        <v>-10.8</v>
       </c>
       <c r="C107">
         <v>106</v>
@@ -1960,10 +1960,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B108">
-        <v>-11.7</v>
+        <v>-10.8</v>
       </c>
       <c r="C108">
         <v>107</v>
@@ -1971,10 +1971,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="B109">
-        <v>-11.8</v>
+        <v>-11.1</v>
       </c>
       <c r="C109">
         <v>108</v>
@@ -1982,10 +1982,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B110">
-        <v>-11.8</v>
+        <v>-11.3</v>
       </c>
       <c r="C110">
         <v>109</v>
@@ -1993,10 +1993,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B111">
-        <v>-12.2</v>
+        <v>-11.3</v>
       </c>
       <c r="C111">
         <v>110</v>
@@ -2004,10 +2004,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B112">
-        <v>-12.3</v>
+        <v>-11.5</v>
       </c>
       <c r="C112">
         <v>111</v>
@@ -2015,10 +2015,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B113">
-        <v>-12.6</v>
+        <v>-11.7</v>
       </c>
       <c r="C113">
         <v>112</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B114">
-        <v>-12.9</v>
+        <v>-13.2</v>
       </c>
       <c r="C114">
         <v>113</v>
@@ -2037,10 +2037,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="B115">
-        <v>-13.4</v>
+        <v>-13.7</v>
       </c>
       <c r="C115">
         <v>114</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="B116">
-        <v>-13.6</v>
+        <v>-13.8</v>
       </c>
       <c r="C116">
         <v>115</v>
@@ -2073,7 +2073,7 @@
         <v>124</v>
       </c>
       <c r="B118">
-        <v>-14.6</v>
+        <v>-14.5</v>
       </c>
       <c r="C118">
         <v>117</v>
@@ -2084,7 +2084,7 @@
         <v>120</v>
       </c>
       <c r="B119">
-        <v>-15.1</v>
+        <v>-14.9</v>
       </c>
       <c r="C119">
         <v>118</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B120">
-        <v>-15.2</v>
+        <v>-15</v>
       </c>
       <c r="C120">
         <v>119</v>
@@ -2103,10 +2103,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B121">
-        <v>-15.3</v>
+        <v>-15.2</v>
       </c>
       <c r="C121">
         <v>120</v>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B122">
-        <v>-16</v>
+        <v>-15.8</v>
       </c>
       <c r="C122">
         <v>121</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B123">
         <v>-16.100000000000001</v>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B124">
-        <v>-16.2</v>
+        <v>-16.399999999999999</v>
       </c>
       <c r="C124">
         <v>123</v>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B125">
-        <v>-16.8</v>
+        <v>-16.600000000000001</v>
       </c>
       <c r="C125">
         <v>124</v>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B126">
-        <v>-16.899999999999999</v>
+        <v>-17.100000000000001</v>
       </c>
       <c r="C126">
         <v>125</v>
@@ -2172,7 +2172,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>-17.899999999999999</v>
+        <v>-17.600000000000001</v>
       </c>
       <c r="C127">
         <v>126</v>
@@ -2183,7 +2183,7 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>-18.2</v>
+        <v>-18.399999999999999</v>
       </c>
       <c r="C128">
         <v>127</v>
@@ -2194,7 +2194,7 @@
         <v>133</v>
       </c>
       <c r="B129">
-        <v>-19.100000000000001</v>
+        <v>-19.2</v>
       </c>
       <c r="C129">
         <v>128</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B130">
-        <v>-19.8</v>
+        <v>-19.600000000000001</v>
       </c>
       <c r="C130">
         <v>129</v>
@@ -2213,10 +2213,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B131">
-        <v>-20</v>
+        <v>-20.100000000000001</v>
       </c>
       <c r="C131">
         <v>130</v>
@@ -2238,7 +2238,7 @@
         <v>134</v>
       </c>
       <c r="B133">
-        <v>-21</v>
+        <v>-20.9</v>
       </c>
       <c r="C133">
         <v>132</v>
@@ -2249,7 +2249,7 @@
         <v>136</v>
       </c>
       <c r="B134">
-        <v>-23.1</v>
+        <v>-22.8</v>
       </c>
       <c r="C134">
         <v>133</v>
@@ -2257,10 +2257,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B135">
-        <v>-23.4</v>
+        <v>-24.3</v>
       </c>
       <c r="C135">
         <v>134</v>
@@ -2268,10 +2268,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B136">
-        <v>-24.3</v>
+        <v>-24.9</v>
       </c>
       <c r="C136">
         <v>135</v>
@@ -2282,7 +2282,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>-28</v>
+        <v>-27.9</v>
       </c>
       <c r="C137">
         <v>136</v>

</xml_diff>

<commit_message>
Week 12 Data Update
</commit_message>
<xml_diff>
--- a/PEAR/kford.xlsx
+++ b/PEAR/kford.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wpars\OneDrive\Documents\Post-School\Family Feud Data\PEAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3C64AF-44FD-46A7-8EB2-55946BA2D542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1849069-E490-44D5-B105-6E54DB50935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -773,7 +773,7 @@
   <dimension ref="A1:C137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127"/>
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,10 +794,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>29.8</v>
+        <v>29.4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -805,10 +805,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>29.6</v>
+        <v>29.2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -819,7 +819,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>25.3</v>
+        <v>25.2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>23.8</v>
+        <v>24.5</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -838,10 +838,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>23.8</v>
+        <v>23.6</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -849,10 +849,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>21.8</v>
+        <v>22.5</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -863,7 +863,7 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>21.6</v>
+        <v>22.4</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -871,10 +871,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>21.6</v>
+        <v>22.1</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -882,10 +882,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B10">
-        <v>20.9</v>
+        <v>21.8</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -896,7 +896,7 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>19.8</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>19.8</v>
@@ -915,10 +915,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>19.5</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -929,7 +929,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>18.100000000000001</v>
+        <v>18.5</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -940,7 +940,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>17.5</v>
+        <v>17.7</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -948,10 +948,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>15.9</v>
+        <v>16.2</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>15.9</v>
@@ -981,10 +981,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B19">
-        <v>15.9</v>
+        <v>15.7</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -992,10 +992,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>15.3</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>15.2</v>
+        <v>14.9</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1017,7 +1017,7 @@
         <v>16</v>
       </c>
       <c r="B22">
-        <v>14.3</v>
+        <v>14.4</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1025,10 +1025,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>14.1</v>
+        <v>13.7</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B24">
-        <v>13.7</v>
+        <v>12.5</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>13.6</v>
+        <v>12.3</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>12.6</v>
+        <v>12.3</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1069,10 +1069,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>12.4</v>
+        <v>12.1</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1080,10 +1080,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B28">
-        <v>12.1</v>
+        <v>11.1</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1091,10 +1091,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>11.9</v>
+        <v>10.6</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B30">
-        <v>10.8</v>
+        <v>10.3</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1113,10 +1113,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B31">
-        <v>10.4</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1124,10 +1124,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32">
-        <v>10.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B33">
-        <v>9.6</v>
+        <v>10</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1146,10 +1146,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B34">
-        <v>9.6</v>
+        <v>9.9</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B35">
-        <v>9.5</v>
+        <v>9.9</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B36">
-        <v>9.1999999999999993</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1179,10 +1179,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B37">
-        <v>8.9</v>
+        <v>9.4</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1190,10 +1190,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B38">
-        <v>8.8000000000000007</v>
+        <v>8.9</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1201,10 +1201,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B39">
-        <v>8.6999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B40">
-        <v>8.6</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B41">
-        <v>8.6</v>
+        <v>8.5</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B42">
-        <v>8.5</v>
+        <v>8.4</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B43">
         <v>8.4</v>
@@ -1256,10 +1256,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B44">
-        <v>8.1999999999999993</v>
+        <v>7.9</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B45">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1278,10 +1278,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B46">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>7.2</v>
+        <v>6.9</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1303,7 +1303,7 @@
         <v>57</v>
       </c>
       <c r="B48">
-        <v>6.5</v>
+        <v>6.2</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -1314,7 +1314,7 @@
         <v>36</v>
       </c>
       <c r="B49">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -1322,10 +1322,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B50">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B51">
         <v>5.7</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B52">
         <v>5</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B53">
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="C53">
         <v>52</v>
@@ -1369,7 +1369,7 @@
         <v>63</v>
       </c>
       <c r="B54">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="C54">
         <v>53</v>
@@ -1377,10 +1377,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B55">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="C55">
         <v>54</v>
@@ -1388,10 +1388,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B56">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="C56">
         <v>55</v>
@@ -1399,10 +1399,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B57">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="C57">
         <v>56</v>
@@ -1410,10 +1410,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B58">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="C58">
         <v>57</v>
@@ -1424,7 +1424,7 @@
         <v>65</v>
       </c>
       <c r="B59">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B60">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="C60">
         <v>59</v>
@@ -1443,10 +1443,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B61">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="C61">
         <v>60</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>1.4</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B63">
         <v>1.3</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B64">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -1487,10 +1487,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B65">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="C65">
         <v>64</v>
@@ -1498,10 +1498,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B66">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="C66">
         <v>65</v>
@@ -1509,10 +1509,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B67">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="C67">
         <v>66</v>
@@ -1520,10 +1520,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B68">
-        <v>-0.7</v>
+        <v>-0.3</v>
       </c>
       <c r="C68">
         <v>67</v>
@@ -1531,10 +1531,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B69">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="C69">
         <v>68</v>
@@ -1542,10 +1542,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B70">
-        <v>-0.8</v>
+        <v>-1.5</v>
       </c>
       <c r="C70">
         <v>69</v>
@@ -1553,10 +1553,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71">
-        <v>-1.6</v>
+        <v>-1.7</v>
       </c>
       <c r="C71">
         <v>70</v>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B73">
-        <v>-1.9</v>
+        <v>-2.1</v>
       </c>
       <c r="C73">
         <v>72</v>
@@ -1589,7 +1589,7 @@
         <v>81</v>
       </c>
       <c r="B74">
-        <v>-2.4</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="C74">
         <v>73</v>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B75">
-        <v>-2.6</v>
+        <v>-2.5</v>
       </c>
       <c r="C75">
         <v>74</v>
@@ -1608,10 +1608,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B76">
-        <v>-2.9</v>
+        <v>-3.1</v>
       </c>
       <c r="C76">
         <v>75</v>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B77">
-        <v>-3.4</v>
+        <v>-3.3</v>
       </c>
       <c r="C77">
         <v>76</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B78">
-        <v>-3.6</v>
+        <v>-3.3</v>
       </c>
       <c r="C78">
         <v>77</v>
@@ -1641,10 +1641,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B79">
-        <v>-3.9</v>
+        <v>-3.4</v>
       </c>
       <c r="C79">
         <v>78</v>
@@ -1652,10 +1652,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B80">
-        <v>-4.0999999999999996</v>
+        <v>-3.9</v>
       </c>
       <c r="C80">
         <v>79</v>
@@ -1663,10 +1663,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B81">
-        <v>-4.5</v>
+        <v>-4.2</v>
       </c>
       <c r="C81">
         <v>80</v>
@@ -1674,10 +1674,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B82">
-        <v>-4.5999999999999996</v>
+        <v>-4.3</v>
       </c>
       <c r="C82">
         <v>81</v>
@@ -1688,7 +1688,7 @@
         <v>71</v>
       </c>
       <c r="B83">
-        <v>-4.7</v>
+        <v>-4.5</v>
       </c>
       <c r="C83">
         <v>82</v>
@@ -1696,10 +1696,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B84">
-        <v>-5</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="C84">
         <v>83</v>
@@ -1707,10 +1707,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B85">
-        <v>-5.2</v>
+        <v>-5.0999999999999996</v>
       </c>
       <c r="C85">
         <v>84</v>
@@ -1718,10 +1718,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
       <c r="B86">
-        <v>-5.4</v>
+        <v>-5.2</v>
       </c>
       <c r="C86">
         <v>85</v>
@@ -1729,10 +1729,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B87">
-        <v>-5.8</v>
+        <v>-5.3</v>
       </c>
       <c r="C87">
         <v>86</v>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="B88">
-        <v>-6.1</v>
+        <v>-5.3</v>
       </c>
       <c r="C88">
         <v>87</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B89">
         <v>-6.1</v>
@@ -1762,10 +1762,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B90">
-        <v>-6.3</v>
+        <v>-6.7</v>
       </c>
       <c r="C90">
         <v>89</v>
@@ -1773,10 +1773,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="B91">
-        <v>-7</v>
+        <v>-6.7</v>
       </c>
       <c r="C91">
         <v>90</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B92">
-        <v>-7.3</v>
+        <v>-6.8</v>
       </c>
       <c r="C92">
         <v>91</v>
@@ -1795,10 +1795,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="B93">
-        <v>-7.4</v>
+        <v>-7.3</v>
       </c>
       <c r="C93">
         <v>92</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>-7.4</v>
@@ -1817,10 +1817,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B95">
-        <v>-7.9</v>
+        <v>-7.5</v>
       </c>
       <c r="C95">
         <v>94</v>
@@ -1828,10 +1828,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B96">
-        <v>-7.9</v>
+        <v>-7.8</v>
       </c>
       <c r="C96">
         <v>95</v>
@@ -1842,7 +1842,7 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>-8</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="C97">
         <v>96</v>
@@ -1861,7 +1861,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B99">
         <v>-8.4</v>
@@ -1875,7 +1875,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>-8.5</v>
+        <v>-8.4</v>
       </c>
       <c r="C100">
         <v>99</v>
@@ -1883,10 +1883,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B101">
-        <v>-9.3000000000000007</v>
+        <v>-8.6</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -1894,10 +1894,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B102">
-        <v>-9.4</v>
+        <v>-10.1</v>
       </c>
       <c r="C102">
         <v>101</v>
@@ -1905,10 +1905,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B103">
-        <v>-9.5</v>
+        <v>-10.199999999999999</v>
       </c>
       <c r="C103">
         <v>102</v>
@@ -1916,10 +1916,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="B104">
-        <v>-10.4</v>
+        <v>-10.5</v>
       </c>
       <c r="C104">
         <v>103</v>
@@ -1927,10 +1927,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B105">
-        <v>-10.7</v>
+        <v>-10.6</v>
       </c>
       <c r="C105">
         <v>104</v>
@@ -1938,10 +1938,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B106">
-        <v>-10.7</v>
+        <v>-11</v>
       </c>
       <c r="C106">
         <v>105</v>
@@ -1949,10 +1949,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B107">
-        <v>-10.8</v>
+        <v>-11</v>
       </c>
       <c r="C107">
         <v>106</v>
@@ -1960,10 +1960,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B108">
-        <v>-10.8</v>
+        <v>-11.1</v>
       </c>
       <c r="C108">
         <v>107</v>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B110">
         <v>-11.3</v>
@@ -1993,10 +1993,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B111">
-        <v>-11.3</v>
+        <v>-11.4</v>
       </c>
       <c r="C111">
         <v>110</v>
@@ -2004,10 +2004,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B112">
-        <v>-11.5</v>
+        <v>-11.8</v>
       </c>
       <c r="C112">
         <v>111</v>
@@ -2015,10 +2015,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="B113">
-        <v>-11.7</v>
+        <v>-12.6</v>
       </c>
       <c r="C113">
         <v>112</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B114">
-        <v>-13.2</v>
+        <v>-13.1</v>
       </c>
       <c r="C114">
         <v>113</v>
@@ -2037,10 +2037,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="B115">
-        <v>-13.7</v>
+        <v>-13.3</v>
       </c>
       <c r="C115">
         <v>114</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B116">
-        <v>-13.8</v>
+        <v>-13.3</v>
       </c>
       <c r="C116">
         <v>115</v>
@@ -2059,10 +2059,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B117">
-        <v>-14.4</v>
+        <v>-14.3</v>
       </c>
       <c r="C117">
         <v>116</v>
@@ -2070,10 +2070,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B118">
-        <v>-14.5</v>
+        <v>-14.3</v>
       </c>
       <c r="C118">
         <v>117</v>
@@ -2081,10 +2081,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B119">
-        <v>-14.9</v>
+        <v>-14.7</v>
       </c>
       <c r="C119">
         <v>118</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B120">
-        <v>-15</v>
+        <v>-14.9</v>
       </c>
       <c r="C120">
         <v>119</v>
@@ -2106,7 +2106,7 @@
         <v>109</v>
       </c>
       <c r="B121">
-        <v>-15.2</v>
+        <v>-15.3</v>
       </c>
       <c r="C121">
         <v>120</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B123">
         <v>-16.100000000000001</v>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B124">
-        <v>-16.399999999999999</v>
+        <v>-16.2</v>
       </c>
       <c r="C124">
         <v>123</v>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B125">
-        <v>-16.600000000000001</v>
+        <v>-16.5</v>
       </c>
       <c r="C125">
         <v>124</v>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B126">
-        <v>-17.100000000000001</v>
+        <v>-17.3</v>
       </c>
       <c r="C126">
         <v>125</v>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B127">
-        <v>-17.600000000000001</v>
+        <v>-17.899999999999999</v>
       </c>
       <c r="C127">
         <v>126</v>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B128">
-        <v>-18.399999999999999</v>
+        <v>-19.100000000000001</v>
       </c>
       <c r="C128">
         <v>127</v>
@@ -2191,10 +2191,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B129">
-        <v>-19.2</v>
+        <v>-19.7</v>
       </c>
       <c r="C129">
         <v>128</v>
@@ -2205,7 +2205,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>-19.600000000000001</v>
+        <v>-20</v>
       </c>
       <c r="C130">
         <v>129</v>
@@ -2227,7 +2227,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>-20.100000000000001</v>
+        <v>-20.2</v>
       </c>
       <c r="C132">
         <v>131</v>
@@ -2235,10 +2235,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B133">
-        <v>-20.9</v>
+        <v>-21.1</v>
       </c>
       <c r="C133">
         <v>132</v>
@@ -2257,10 +2257,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B135">
-        <v>-24.3</v>
+        <v>-23</v>
       </c>
       <c r="C135">
         <v>134</v>
@@ -2268,10 +2268,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B136">
-        <v>-24.9</v>
+        <v>-23.9</v>
       </c>
       <c r="C136">
         <v>135</v>
@@ -2282,7 +2282,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>-27.9</v>
+        <v>-30</v>
       </c>
       <c r="C137">
         <v>136</v>

</xml_diff>